<commit_message>
Update XLSX + Update XML
</commit_message>
<xml_diff>
--- a/httpget/List File.xlsx
+++ b/httpget/List File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\script-nsg\httpget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{384A4B84-0BDA-483F-A416-22CE97214BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6098CE44-4DC9-42BB-84A5-279B2BE242E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{DC6502BA-425D-411E-B718-7BD70301C676}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
   <si>
     <t>Country</t>
   </si>
@@ -222,6 +222,60 @@
   </si>
   <si>
     <t>Cloudflare_Blender_CDN.xml</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Consortium GARR</t>
+  </si>
+  <si>
+    <t>100Gbps</t>
+  </si>
+  <si>
+    <t>Consortium GARR_100Gbps_IT.xml</t>
+  </si>
+  <si>
+    <t>DigitalOcean Spaces</t>
+  </si>
+  <si>
+    <t>DigitalOcean Spaces_Germany_Frankfurt_DE.xml</t>
+  </si>
+  <si>
+    <t>DZ</t>
+  </si>
+  <si>
+    <t>Djezzy Alger</t>
+  </si>
+  <si>
+    <t>1Gbps</t>
+  </si>
+  <si>
+    <t>Djezzy Alger_1Gbps_DZ.xml</t>
+  </si>
+  <si>
+    <t>Djezzy Annaba</t>
+  </si>
+  <si>
+    <t>Djezzy Annaba_1Gbps_DZ.xml</t>
+  </si>
+  <si>
+    <t>Google Cloud Storage</t>
+  </si>
+  <si>
+    <t>Google Cloud Storage_CDN.xml</t>
+  </si>
+  <si>
+    <t>Green Data</t>
+  </si>
+  <si>
+    <t>Green Data_10Gbps_FR.xml</t>
+  </si>
+  <si>
+    <t>HessFR</t>
+  </si>
+  <si>
+    <t>HessFR_10Gbps_FR.xml</t>
   </si>
 </sst>
 </file>
@@ -263,7 +317,38 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -593,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C18607A-68F6-4C8B-BF40-82CCB3747CF3}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,16 +777,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
@@ -709,16 +794,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
@@ -726,16 +811,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
@@ -746,13 +831,13 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
@@ -763,13 +848,13 @@
         <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
         <v>15</v>
@@ -780,13 +865,13 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
@@ -797,13 +882,13 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
@@ -814,13 +899,13 @@
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>
@@ -831,13 +916,13 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
         <v>15</v>
@@ -848,13 +933,13 @@
         <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
@@ -862,16 +947,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
@@ -879,16 +964,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
@@ -896,16 +981,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
@@ -913,16 +998,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="E19" t="s">
         <v>15</v>
@@ -930,16 +1015,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="E20" t="s">
         <v>15</v>
@@ -947,16 +1032,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s">
         <v>15</v>
@@ -964,22 +1049,149 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
         <v>28</v>
       </c>
       <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
         <v>61</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update XLSX + Correction name SFR Rennes + Remove doublon
</commit_message>
<xml_diff>
--- a/httpget/List File.xlsx
+++ b/httpget/List File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\script-nsg\httpget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7455668E-1F47-4E8C-BCB3-529703765472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D981607-BDB8-46E2-836F-7C99BD765D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{DC6502BA-425D-411E-B718-7BD70301C676}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="188">
   <si>
     <t>Country</t>
   </si>
@@ -453,6 +453,153 @@
   </si>
   <si>
     <t>Orange FR Rennes_10Gbps_FR.xml</t>
+  </si>
+  <si>
+    <t>Orange FR Strasbourg</t>
+  </si>
+  <si>
+    <t>Orange FR Strasbourg_10Gbps_FR.xml</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>Orange MA Casablanca</t>
+  </si>
+  <si>
+    <t>Orange MA Casablanca_10Gbps_MA.xml</t>
+  </si>
+  <si>
+    <t>Orange MA Rabat</t>
+  </si>
+  <si>
+    <t>Orange MA Rabat_10Gbps_MA.xml</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>Orange SN</t>
+  </si>
+  <si>
+    <t>Orange SN_10Gbps_SN.xml</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>Orange TN</t>
+  </si>
+  <si>
+    <t>Orange TN_1Gbps_TN.xml</t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>Outremer Telecom</t>
+  </si>
+  <si>
+    <t>Outremer Telecom_1Gbps_MU.xml</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>OVH AU SYD</t>
+  </si>
+  <si>
+    <t>OVH AU SYD_10Gbps_AU.xml</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>OVH CA BHS_10Gbps_CA.xml</t>
+  </si>
+  <si>
+    <t>OVH CA BHS</t>
+  </si>
+  <si>
+    <t>OVH FR GRA</t>
+  </si>
+  <si>
+    <t>OVH FR GRA_10Gbps_FR.xml</t>
+  </si>
+  <si>
+    <t>OVH FR RBX</t>
+  </si>
+  <si>
+    <t>OVH FR RBX_10Gbps_FR.xml</t>
+  </si>
+  <si>
+    <t>OVH FR SBG</t>
+  </si>
+  <si>
+    <t>OVH FR SBG_10Gbps_FR.xml</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>OVH IN BOM</t>
+  </si>
+  <si>
+    <t>OVH IN BOM_10Gbps_IN.xml</t>
+  </si>
+  <si>
+    <t>OVH SG</t>
+  </si>
+  <si>
+    <t>OVH SG_10Gbps_SG.xml</t>
+  </si>
+  <si>
+    <t>OVH UK ERI</t>
+  </si>
+  <si>
+    <t>OVH UK ERI_10Gbps_UK.xml</t>
+  </si>
+  <si>
+    <t>OVH HIL</t>
+  </si>
+  <si>
+    <t>OVH US HIL_10Gbps_USA, Hillsboro.xml</t>
+  </si>
+  <si>
+    <t>OVH VIN</t>
+  </si>
+  <si>
+    <t>OVH USA VIN_10Gbps_US.xml</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>Salt CH_100Gbps_CH.xml</t>
+  </si>
+  <si>
+    <t>Scaleway Cubic</t>
+  </si>
+  <si>
+    <t>Scaleway_ Cubic_10Gbps_NL.xml</t>
+  </si>
+  <si>
+    <t>Scaleway Cubic IPv4</t>
+  </si>
+  <si>
+    <t>Scaleway_ Cubic_IPv4_100Gbps_FR.xml</t>
+  </si>
+  <si>
+    <t>Scaleway Cubic IPv6</t>
+  </si>
+  <si>
+    <t>Scaleway_ Cubic_IPv6_100Gbps_FR.xml</t>
+  </si>
+  <si>
+    <t>Scaleway Cubic DC3 BBR</t>
+  </si>
+  <si>
+    <t>Scaleway_ DC3_BBR_10Gbps_FR.xml</t>
   </si>
 </sst>
 </file>
@@ -845,10 +992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C18607A-68F6-4C8B-BF40-82CCB3747CF3}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,16 +1057,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>157</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -927,16 +1074,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>160</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>107</v>
+        <v>159</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
@@ -944,16 +1091,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
@@ -961,16 +1108,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>178</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>179</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
@@ -978,16 +1125,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
@@ -995,16 +1142,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
@@ -1012,16 +1159,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
         <v>15</v>
@@ -1029,16 +1176,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
@@ -1046,16 +1193,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
@@ -1063,16 +1210,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
-        <v>114</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>
@@ -1083,13 +1230,13 @@
         <v>108</v>
       </c>
       <c r="B14" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="D14" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E14" t="s">
         <v>15</v>
@@ -1100,13 +1247,13 @@
         <v>108</v>
       </c>
       <c r="B15" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C15" t="s">
         <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
@@ -1114,16 +1261,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
@@ -1131,16 +1278,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>115</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>116</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
@@ -1148,16 +1295,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
@@ -1165,16 +1312,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="E19" t="s">
         <v>15</v>
@@ -1185,13 +1332,13 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E20" t="s">
         <v>15</v>
@@ -1202,13 +1349,13 @@
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
         <v>15</v>
@@ -1219,13 +1366,13 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E22" t="s">
         <v>15</v>
@@ -1236,13 +1383,13 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E23" t="s">
         <v>15</v>
@@ -1253,13 +1400,13 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
@@ -1270,13 +1417,13 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
@@ -1287,13 +1434,13 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E26" t="s">
         <v>15</v>
@@ -1304,13 +1451,13 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="E27" t="s">
         <v>15</v>
@@ -1321,13 +1468,13 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
@@ -1338,13 +1485,13 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="E29" t="s">
         <v>15</v>
@@ -1355,13 +1502,13 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
@@ -1372,13 +1519,13 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="E31" t="s">
         <v>15</v>
@@ -1389,13 +1536,13 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="E32" t="s">
         <v>15</v>
@@ -1406,13 +1553,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="E33" t="s">
         <v>15</v>
@@ -1423,13 +1570,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D34" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="E34" t="s">
         <v>15</v>
@@ -1440,13 +1587,13 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E35" t="s">
         <v>15</v>
@@ -1457,13 +1604,13 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E36" t="s">
         <v>15</v>
@@ -1474,13 +1621,13 @@
         <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E37" t="s">
         <v>15</v>
@@ -1491,13 +1638,13 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="E38" t="s">
         <v>15</v>
@@ -1508,13 +1655,13 @@
         <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E39" t="s">
         <v>15</v>
@@ -1525,13 +1672,13 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E40" t="s">
         <v>15</v>
@@ -1542,13 +1689,13 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E41" t="s">
         <v>15</v>
@@ -1556,16 +1703,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>133</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>19</v>
+        <v>134</v>
       </c>
       <c r="E42" t="s">
         <v>15</v>
@@ -1573,16 +1720,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>27</v>
+        <v>135</v>
       </c>
       <c r="C43" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>26</v>
+        <v>136</v>
       </c>
       <c r="E43" t="s">
         <v>15</v>
@@ -1590,16 +1737,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>63</v>
+        <v>137</v>
       </c>
       <c r="C44" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="D44" t="s">
-        <v>65</v>
+        <v>138</v>
       </c>
       <c r="E44" t="s">
         <v>15</v>
@@ -1607,16 +1754,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>139</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="E45" t="s">
         <v>15</v>
@@ -1624,16 +1771,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>161</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
       </c>
       <c r="D46" t="s">
-        <v>8</v>
+        <v>162</v>
       </c>
       <c r="E46" t="s">
         <v>15</v>
@@ -1641,16 +1788,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>163</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
       </c>
       <c r="D47" t="s">
-        <v>104</v>
+        <v>164</v>
       </c>
       <c r="E47" t="s">
         <v>15</v>
@@ -1658,16 +1805,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B48" t="s">
-        <v>36</v>
+        <v>165</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>37</v>
+        <v>166</v>
       </c>
       <c r="E48" t="s">
         <v>15</v>
@@ -1675,16 +1822,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B49" t="s">
-        <v>24</v>
+        <v>182</v>
       </c>
       <c r="C49" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="D49" t="s">
-        <v>26</v>
+        <v>183</v>
       </c>
       <c r="E49" t="s">
         <v>15</v>
@@ -1692,16 +1839,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="B50" t="s">
-        <v>90</v>
+        <v>184</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D50" t="s">
-        <v>91</v>
+        <v>185</v>
       </c>
       <c r="E50" t="s">
         <v>15</v>
@@ -1709,16 +1856,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B51" t="s">
-        <v>30</v>
+        <v>186</v>
       </c>
       <c r="C51" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D51" t="s">
-        <v>31</v>
+        <v>187</v>
       </c>
       <c r="E51" t="s">
         <v>15</v>
@@ -1726,16 +1873,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B52" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
       <c r="C52" t="s">
         <v>6</v>
       </c>
       <c r="D52" t="s">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="E52" t="s">
         <v>15</v>
@@ -1743,16 +1890,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B53" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D53" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="E53" t="s">
         <v>15</v>
@@ -1760,16 +1907,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>172</v>
       </c>
       <c r="C54" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D54" t="s">
-        <v>61</v>
+        <v>173</v>
       </c>
       <c r="E54" t="s">
         <v>15</v>
@@ -1777,16 +1924,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>167</v>
       </c>
       <c r="B55" t="s">
-        <v>74</v>
+        <v>168</v>
       </c>
       <c r="C55" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>75</v>
+        <v>169</v>
       </c>
       <c r="E55" t="s">
         <v>15</v>
@@ -1794,18 +1941,375 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" t="s">
+        <v>64</v>
+      </c>
+      <c r="D56" t="s">
+        <v>65</v>
+      </c>
+      <c r="E56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>141</v>
+      </c>
+      <c r="B57" t="s">
+        <v>142</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" t="s">
+        <v>143</v>
+      </c>
+      <c r="E57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>141</v>
+      </c>
+      <c r="B58" t="s">
+        <v>144</v>
+      </c>
+      <c r="C58" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" t="s">
+        <v>145</v>
+      </c>
+      <c r="E58" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>100</v>
+      </c>
+      <c r="B59" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" t="s">
+        <v>102</v>
+      </c>
+      <c r="E59" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>152</v>
+      </c>
+      <c r="B60" t="s">
+        <v>153</v>
+      </c>
+      <c r="C60" t="s">
+        <v>70</v>
+      </c>
+      <c r="D60" t="s">
+        <v>154</v>
+      </c>
+      <c r="E60" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62" t="s">
+        <v>103</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" t="s">
+        <v>104</v>
+      </c>
+      <c r="E62" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63" t="s">
+        <v>180</v>
+      </c>
+      <c r="C63" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" t="s">
+        <v>181</v>
+      </c>
+      <c r="E63" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" t="s">
+        <v>36</v>
+      </c>
+      <c r="C64" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" t="s">
+        <v>37</v>
+      </c>
+      <c r="E64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>23</v>
+      </c>
+      <c r="B65" t="s">
+        <v>24</v>
+      </c>
+      <c r="C65" t="s">
+        <v>25</v>
+      </c>
+      <c r="D65" t="s">
+        <v>26</v>
+      </c>
+      <c r="E65" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>89</v>
+      </c>
+      <c r="B66" t="s">
+        <v>90</v>
+      </c>
+      <c r="C66" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" t="s">
+        <v>91</v>
+      </c>
+      <c r="E66" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>89</v>
+      </c>
+      <c r="B67" t="s">
+        <v>170</v>
+      </c>
+      <c r="C67" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" t="s">
+        <v>171</v>
+      </c>
+      <c r="E67" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>146</v>
+      </c>
+      <c r="B68" t="s">
+        <v>147</v>
+      </c>
+      <c r="C68" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" t="s">
+        <v>148</v>
+      </c>
+      <c r="E68" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>149</v>
+      </c>
+      <c r="B69" t="s">
+        <v>150</v>
+      </c>
+      <c r="C69" t="s">
+        <v>70</v>
+      </c>
+      <c r="D69" t="s">
+        <v>151</v>
+      </c>
+      <c r="E69" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>29</v>
+      </c>
+      <c r="B70" t="s">
+        <v>30</v>
+      </c>
+      <c r="C70" t="s">
+        <v>28</v>
+      </c>
+      <c r="D70" t="s">
+        <v>31</v>
+      </c>
+      <c r="E70" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>29</v>
+      </c>
+      <c r="B71" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" t="s">
+        <v>81</v>
+      </c>
+      <c r="E71" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>29</v>
+      </c>
+      <c r="B72" t="s">
+        <v>87</v>
+      </c>
+      <c r="C72" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" t="s">
+        <v>88</v>
+      </c>
+      <c r="E72" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>29</v>
+      </c>
+      <c r="B73" t="s">
+        <v>174</v>
+      </c>
+      <c r="C73" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" t="s">
+        <v>175</v>
+      </c>
+      <c r="E73" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>29</v>
+      </c>
+      <c r="B74" t="s">
+        <v>176</v>
+      </c>
+      <c r="C74" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" t="s">
+        <v>177</v>
+      </c>
+      <c r="E74" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>59</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B75" t="s">
+        <v>60</v>
+      </c>
+      <c r="C75" t="s">
+        <v>28</v>
+      </c>
+      <c r="D75" t="s">
+        <v>61</v>
+      </c>
+      <c r="E75" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>59</v>
+      </c>
+      <c r="B76" t="s">
+        <v>74</v>
+      </c>
+      <c r="C76" t="s">
+        <v>28</v>
+      </c>
+      <c r="D76" t="s">
+        <v>75</v>
+      </c>
+      <c r="E76" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>59</v>
+      </c>
+      <c r="B77" t="s">
         <v>96</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C77" t="s">
         <v>28</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D77" t="s">
         <v>97</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E77" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Spain to the Website
</commit_message>
<xml_diff>
--- a/httpget/List File.xlsx
+++ b/httpget/List File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\script-nsg\httpget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465335A3-45CC-40FA-8093-C3BF9AB7E624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A117EE-843F-470C-9E6B-C449393313AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{DC6502BA-425D-411E-B718-7BD70301C676}"/>
   </bookViews>
@@ -365,9 +365,6 @@
     <t>Orange ES Barcelona</t>
   </si>
   <si>
-    <t>Orange ES Barcelona_100Gbps_ES</t>
-  </si>
-  <si>
     <t>Orange ES Bilbao</t>
   </si>
   <si>
@@ -380,15 +377,9 @@
     <t>Orange ES Madrid_100Gbps_ES.xml</t>
   </si>
   <si>
-    <t>Orange Sevilla</t>
-  </si>
-  <si>
     <t>Orange ES Sevilla_20Gbps_ES.xml</t>
   </si>
   <si>
-    <t>Orange Valladolid</t>
-  </si>
-  <si>
     <t>Orange ES Valladolid_20Gbps_ES.xml</t>
   </si>
   <si>
@@ -708,6 +699,15 @@
   </si>
   <si>
     <t>31173 Services AB_10Gbps_Zurich_CH.xml</t>
+  </si>
+  <si>
+    <t>Orange ES Sevilla</t>
+  </si>
+  <si>
+    <t>Orange ES Valladolid</t>
+  </si>
+  <si>
+    <t>Orange ES Barcelona_100Gbps_ES.xml</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1103,7 @@
   <dimension ref="A1:E94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E9"/>
+      <selection activeCell="E15" sqref="E15:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,13 +1168,13 @@
         <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -1182,16 +1182,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -1199,16 +1199,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C6" t="s">
         <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -1216,16 +1216,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -1242,7 +1242,7 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -1253,13 +1253,13 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C9" t="s">
         <v>63</v>
       </c>
       <c r="D9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -1347,7 +1347,7 @@
         <v>70</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1364,7 +1364,7 @@
         <v>72</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1378,10 +1378,10 @@
         <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>109</v>
+        <v>223</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1389,16 +1389,16 @@
         <v>107</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1406,16 +1406,16 @@
         <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C18" t="s">
         <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1423,16 +1423,16 @@
         <v>107</v>
       </c>
       <c r="B19" t="s">
-        <v>114</v>
+        <v>221</v>
       </c>
       <c r="C19" t="s">
         <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1440,16 +1440,16 @@
         <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>222</v>
       </c>
       <c r="C20" t="s">
         <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1729,13 +1729,13 @@
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E37" t="s">
         <v>15</v>
@@ -1746,13 +1746,13 @@
         <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E38" t="s">
         <v>15</v>
@@ -1763,13 +1763,13 @@
         <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E39" t="s">
         <v>15</v>
@@ -1780,13 +1780,13 @@
         <v>31</v>
       </c>
       <c r="B40" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E40" t="s">
         <v>15</v>
@@ -1797,13 +1797,13 @@
         <v>31</v>
       </c>
       <c r="B41" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E41" t="s">
         <v>15</v>
@@ -1814,13 +1814,13 @@
         <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E42" t="s">
         <v>15</v>
@@ -1831,13 +1831,13 @@
         <v>31</v>
       </c>
       <c r="B43" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E43" t="s">
         <v>15</v>
@@ -1848,13 +1848,13 @@
         <v>31</v>
       </c>
       <c r="B44" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
       </c>
       <c r="D44" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E44" t="s">
         <v>15</v>
@@ -1865,13 +1865,13 @@
         <v>31</v>
       </c>
       <c r="B45" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E45" t="s">
         <v>15</v>
@@ -1882,13 +1882,13 @@
         <v>31</v>
       </c>
       <c r="B46" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
       </c>
       <c r="D46" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E46" t="s">
         <v>15</v>
@@ -1899,13 +1899,13 @@
         <v>31</v>
       </c>
       <c r="B47" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
       </c>
       <c r="D47" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E47" t="s">
         <v>15</v>
@@ -1916,13 +1916,13 @@
         <v>31</v>
       </c>
       <c r="B48" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E48" t="s">
         <v>15</v>
@@ -1933,13 +1933,13 @@
         <v>31</v>
       </c>
       <c r="B49" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C49" t="s">
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E49" t="s">
         <v>15</v>
@@ -1950,13 +1950,13 @@
         <v>31</v>
       </c>
       <c r="B50" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C50" t="s">
         <v>6</v>
       </c>
       <c r="D50" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E50" t="s">
         <v>15</v>
@@ -1967,13 +1967,13 @@
         <v>31</v>
       </c>
       <c r="B51" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C51" t="s">
         <v>63</v>
       </c>
       <c r="D51" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E51" t="s">
         <v>15</v>
@@ -1984,13 +1984,13 @@
         <v>31</v>
       </c>
       <c r="B52" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C52" t="s">
         <v>63</v>
       </c>
       <c r="D52" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E52" t="s">
         <v>15</v>
@@ -2001,13 +2001,13 @@
         <v>31</v>
       </c>
       <c r="B53" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C53" t="s">
         <v>6</v>
       </c>
       <c r="D53" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E53" t="s">
         <v>15</v>
@@ -2018,13 +2018,13 @@
         <v>31</v>
       </c>
       <c r="B54" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
       </c>
       <c r="D54" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E54" t="s">
         <v>15</v>
@@ -2035,13 +2035,13 @@
         <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E55" t="s">
         <v>15</v>
@@ -2052,13 +2052,13 @@
         <v>31</v>
       </c>
       <c r="B56" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
       </c>
       <c r="D56" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E56" t="s">
         <v>15</v>
@@ -2069,13 +2069,13 @@
         <v>31</v>
       </c>
       <c r="B57" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
       </c>
       <c r="D57" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E57" t="s">
         <v>15</v>
@@ -2086,13 +2086,13 @@
         <v>31</v>
       </c>
       <c r="B58" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C58" t="s">
         <v>6</v>
       </c>
       <c r="D58" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E58" t="s">
         <v>15</v>
@@ -2103,13 +2103,13 @@
         <v>31</v>
       </c>
       <c r="B59" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C59" t="s">
         <v>6</v>
       </c>
       <c r="D59" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E59" t="s">
         <v>15</v>
@@ -2120,13 +2120,13 @@
         <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C60" t="s">
         <v>6</v>
       </c>
       <c r="D60" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E60" t="s">
         <v>15</v>
@@ -2137,13 +2137,13 @@
         <v>31</v>
       </c>
       <c r="B61" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C61" t="s">
         <v>6</v>
       </c>
       <c r="D61" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E61" t="s">
         <v>15</v>
@@ -2154,13 +2154,13 @@
         <v>31</v>
       </c>
       <c r="B62" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C62" t="s">
         <v>63</v>
       </c>
       <c r="D62" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E62" t="s">
         <v>15</v>
@@ -2171,13 +2171,13 @@
         <v>31</v>
       </c>
       <c r="B63" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C63" t="s">
         <v>6</v>
       </c>
       <c r="D63" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E63" t="s">
         <v>15</v>
@@ -2222,13 +2222,13 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C66" t="s">
         <v>6</v>
       </c>
       <c r="D66" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E66" t="s">
         <v>15</v>
@@ -2236,16 +2236,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B67" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C67" t="s">
         <v>6</v>
       </c>
       <c r="D67" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E67" t="s">
         <v>15</v>
@@ -2270,16 +2270,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B69" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C69" t="s">
         <v>6</v>
       </c>
       <c r="D69" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E69" t="s">
         <v>15</v>
@@ -2287,16 +2287,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B70" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C70" t="s">
         <v>6</v>
       </c>
       <c r="D70" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E70" t="s">
         <v>15</v>
@@ -2304,16 +2304,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>137</v>
+      </c>
+      <c r="B71" t="s">
         <v>140</v>
       </c>
-      <c r="B71" t="s">
-        <v>143</v>
-      </c>
       <c r="C71" t="s">
         <v>6</v>
       </c>
       <c r="D71" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E71" t="s">
         <v>15</v>
@@ -2338,16 +2338,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B73" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C73" t="s">
         <v>69</v>
       </c>
       <c r="D73" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E73" t="s">
         <v>15</v>
@@ -2392,13 +2392,13 @@
         <v>10</v>
       </c>
       <c r="B76" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
       </c>
       <c r="D76" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E76" t="s">
         <v>15</v>
@@ -2409,13 +2409,13 @@
         <v>10</v>
       </c>
       <c r="B77" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
       </c>
       <c r="D77" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E77" t="s">
         <v>15</v>
@@ -2460,13 +2460,13 @@
         <v>22</v>
       </c>
       <c r="B80" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
       </c>
       <c r="D80" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E80" t="s">
         <v>15</v>
@@ -2477,13 +2477,13 @@
         <v>22</v>
       </c>
       <c r="B81" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C81" t="s">
         <v>6</v>
       </c>
       <c r="D81" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E81" t="s">
         <v>15</v>
@@ -2511,13 +2511,13 @@
         <v>88</v>
       </c>
       <c r="B83" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C83" t="s">
         <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E83" t="s">
         <v>15</v>
@@ -2528,13 +2528,13 @@
         <v>88</v>
       </c>
       <c r="B84" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C84" t="s">
         <v>69</v>
       </c>
       <c r="D84" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E84" t="s">
         <v>15</v>
@@ -2542,16 +2542,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B85" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C85" t="s">
         <v>6</v>
       </c>
       <c r="D85" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E85" t="s">
         <v>15</v>
@@ -2559,16 +2559,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B86" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C86" t="s">
         <v>69</v>
       </c>
       <c r="D86" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E86" t="s">
         <v>15</v>
@@ -2630,13 +2630,13 @@
         <v>28</v>
       </c>
       <c r="B90" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C90" t="s">
         <v>6</v>
       </c>
       <c r="D90" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E90" t="s">
         <v>15</v>
@@ -2647,13 +2647,13 @@
         <v>28</v>
       </c>
       <c r="B91" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C91" t="s">
         <v>6</v>
       </c>
       <c r="D91" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E91" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Add France into website
</commit_message>
<xml_diff>
--- a/httpget/List File.xlsx
+++ b/httpget/List File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\script-nsg\httpget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F810DA-9841-4FB6-A2B6-8912A9CAD29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEBA293-40C4-4A15-B14A-F2CA47350320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{DC6502BA-425D-411E-B718-7BD70301C676}"/>
   </bookViews>
@@ -191,9 +191,6 @@
     <t>Bouygues Telecom Strasbourg_10Gbps_FR.xml</t>
   </si>
   <si>
-    <t>Bouygue Telecom Toulouse</t>
-  </si>
-  <si>
     <t>Bouygues Telecom_10Gbps_FR.xml</t>
   </si>
   <si>
@@ -584,9 +581,6 @@
     <t>Scaleway_ Cubic_IPv6_100Gbps_FR.xml</t>
   </si>
   <si>
-    <t>Scaleway Cubic DC3 BBR</t>
-  </si>
-  <si>
     <t>Scaleway_ DC3_BBR_10Gbps_FR.xml</t>
   </si>
   <si>
@@ -708,6 +702,12 @@
   </si>
   <si>
     <t>Orange ES Barcelona_100Gbps_ES.xml</t>
+  </si>
+  <si>
+    <t>Bouygue Telecoms Toulouse</t>
+  </si>
+  <si>
+    <t>Scaleway DC3 BBR</t>
   </si>
 </sst>
 </file>
@@ -1102,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C18607A-68F6-4C8B-BF40-82CCB3747CF3}">
   <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47:E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,16 +1148,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
         <v>55</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>56</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>57</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -1165,16 +1165,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -1182,16 +1182,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" t="s">
         <v>151</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
         <v>152</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>153</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -1199,16 +1199,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s">
         <v>217</v>
-      </c>
-      <c r="B6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" t="s">
-        <v>219</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -1216,16 +1216,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
         <v>154</v>
-      </c>
-      <c r="B7" t="s">
-        <v>156</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>155</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -1242,7 +1242,7 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -1253,13 +1253,13 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" t="s">
         <v>174</v>
-      </c>
-      <c r="C9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" t="s">
-        <v>175</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -1267,16 +1267,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" t="s">
         <v>104</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" t="s">
         <v>105</v>
-      </c>
-      <c r="C10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" t="s">
-        <v>106</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -1304,13 +1304,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
@@ -1321,13 +1321,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
         <v>81</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>82</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -1335,16 +1335,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" t="s">
         <v>67</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>68</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>69</v>
-      </c>
-      <c r="D14" t="s">
-        <v>70</v>
       </c>
       <c r="E14" t="s">
         <v>14</v>
@@ -1352,16 +1352,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" t="s">
         <v>71</v>
-      </c>
-      <c r="C15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" t="s">
-        <v>72</v>
       </c>
       <c r="E15" t="s">
         <v>14</v>
@@ -1369,16 +1369,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" t="s">
         <v>107</v>
       </c>
-      <c r="B16" t="s">
-        <v>108</v>
-      </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E16" t="s">
         <v>14</v>
@@ -1386,16 +1386,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E17" t="s">
         <v>14</v>
@@ -1403,16 +1403,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" t="s">
         <v>111</v>
-      </c>
-      <c r="C18" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" t="s">
-        <v>112</v>
       </c>
       <c r="E18" t="s">
         <v>14</v>
@@ -1420,16 +1420,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C19" t="s">
         <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E19" t="s">
         <v>14</v>
@@ -1437,16 +1437,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B20" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C20" t="s">
         <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E20" t="s">
         <v>14</v>
@@ -1454,16 +1454,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
         <v>83</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
         <v>84</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>85</v>
       </c>
       <c r="E21" t="s">
         <v>14</v>
@@ -1483,7 +1483,7 @@
         <v>34</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1500,7 +1500,7 @@
         <v>38</v>
       </c>
       <c r="E23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1517,7 +1517,7 @@
         <v>40</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1534,7 +1534,7 @@
         <v>44</v>
       </c>
       <c r="E25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1542,16 +1542,16 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
         <v>53</v>
       </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" t="s">
-        <v>54</v>
-      </c>
       <c r="E26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1568,7 +1568,7 @@
         <v>45</v>
       </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1585,7 +1585,7 @@
         <v>46</v>
       </c>
       <c r="E28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1602,7 +1602,7 @@
         <v>47</v>
       </c>
       <c r="E29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1619,7 +1619,7 @@
         <v>50</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1627,16 +1627,16 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
+        <v>222</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
         <v>51</v>
       </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" t="s">
-        <v>52</v>
-      </c>
       <c r="E31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1644,16 +1644,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
         <v>75</v>
       </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" t="s">
-        <v>76</v>
-      </c>
       <c r="E32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1661,16 +1661,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
         <v>77</v>
       </c>
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" t="s">
-        <v>78</v>
-      </c>
       <c r="E33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1678,16 +1678,16 @@
         <v>31</v>
       </c>
       <c r="B34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
         <v>91</v>
       </c>
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" t="s">
-        <v>92</v>
-      </c>
       <c r="E34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1695,16 +1695,16 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
         <v>93</v>
       </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" t="s">
-        <v>94</v>
-      </c>
       <c r="E35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1712,16 +1712,16 @@
         <v>31</v>
       </c>
       <c r="B36" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" t="s">
         <v>97</v>
       </c>
-      <c r="C36" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" t="s">
-        <v>98</v>
-      </c>
       <c r="E36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1729,16 +1729,16 @@
         <v>31</v>
       </c>
       <c r="B37" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
         <v>117</v>
       </c>
-      <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" t="s">
-        <v>118</v>
-      </c>
       <c r="E37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1746,16 +1746,16 @@
         <v>31</v>
       </c>
       <c r="B38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
         <v>119</v>
       </c>
-      <c r="C38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" t="s">
-        <v>120</v>
-      </c>
       <c r="E38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1763,16 +1763,16 @@
         <v>31</v>
       </c>
       <c r="B39" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
         <v>121</v>
       </c>
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" t="s">
-        <v>122</v>
-      </c>
       <c r="E39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1780,16 +1780,16 @@
         <v>31</v>
       </c>
       <c r="B40" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
         <v>115</v>
       </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" t="s">
-        <v>116</v>
-      </c>
       <c r="E40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1797,16 +1797,16 @@
         <v>31</v>
       </c>
       <c r="B41" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
         <v>123</v>
       </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" t="s">
-        <v>124</v>
-      </c>
       <c r="E41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1814,16 +1814,16 @@
         <v>31</v>
       </c>
       <c r="B42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
         <v>125</v>
       </c>
-      <c r="C42" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" t="s">
-        <v>126</v>
-      </c>
       <c r="E42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1831,16 +1831,16 @@
         <v>31</v>
       </c>
       <c r="B43" t="s">
+        <v>126</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
         <v>127</v>
       </c>
-      <c r="C43" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" t="s">
-        <v>128</v>
-      </c>
       <c r="E43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1848,16 +1848,16 @@
         <v>31</v>
       </c>
       <c r="B44" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
         <v>129</v>
       </c>
-      <c r="C44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" t="s">
-        <v>130</v>
-      </c>
       <c r="E44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1865,16 +1865,16 @@
         <v>31</v>
       </c>
       <c r="B45" t="s">
+        <v>130</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
         <v>131</v>
       </c>
-      <c r="C45" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" t="s">
-        <v>132</v>
-      </c>
       <c r="E45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1882,16 +1882,16 @@
         <v>31</v>
       </c>
       <c r="B46" t="s">
+        <v>132</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
         <v>133</v>
       </c>
-      <c r="C46" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" t="s">
-        <v>134</v>
-      </c>
       <c r="E46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1899,16 +1899,16 @@
         <v>31</v>
       </c>
       <c r="B47" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
         <v>135</v>
       </c>
-      <c r="C47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" t="s">
-        <v>136</v>
-      </c>
       <c r="E47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1916,16 +1916,16 @@
         <v>31</v>
       </c>
       <c r="B48" t="s">
+        <v>156</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
         <v>157</v>
       </c>
-      <c r="C48" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" t="s">
-        <v>158</v>
-      </c>
       <c r="E48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1933,16 +1933,16 @@
         <v>31</v>
       </c>
       <c r="B49" t="s">
+        <v>158</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
         <v>159</v>
       </c>
-      <c r="C49" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" t="s">
-        <v>160</v>
-      </c>
       <c r="E49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1950,16 +1950,16 @@
         <v>31</v>
       </c>
       <c r="B50" t="s">
+        <v>160</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s">
         <v>161</v>
       </c>
-      <c r="C50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" t="s">
-        <v>162</v>
-      </c>
       <c r="E50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1967,16 +1967,16 @@
         <v>31</v>
       </c>
       <c r="B51" t="s">
+        <v>177</v>
+      </c>
+      <c r="C51" t="s">
+        <v>62</v>
+      </c>
+      <c r="D51" t="s">
         <v>178</v>
       </c>
-      <c r="C51" t="s">
-        <v>63</v>
-      </c>
-      <c r="D51" t="s">
-        <v>179</v>
-      </c>
       <c r="E51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1984,16 +1984,16 @@
         <v>31</v>
       </c>
       <c r="B52" t="s">
+        <v>179</v>
+      </c>
+      <c r="C52" t="s">
+        <v>62</v>
+      </c>
+      <c r="D52" t="s">
         <v>180</v>
       </c>
-      <c r="C52" t="s">
-        <v>63</v>
-      </c>
-      <c r="D52" t="s">
-        <v>181</v>
-      </c>
       <c r="E52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2001,16 +2001,16 @@
         <v>31</v>
       </c>
       <c r="B53" t="s">
-        <v>182</v>
+        <v>223</v>
       </c>
       <c r="C53" t="s">
         <v>6</v>
       </c>
       <c r="D53" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E53" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2018,16 +2018,16 @@
         <v>31</v>
       </c>
       <c r="B54" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
       </c>
       <c r="D54" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E54" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2035,16 +2035,16 @@
         <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2052,16 +2052,16 @@
         <v>31</v>
       </c>
       <c r="B56" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
       </c>
       <c r="D56" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2069,16 +2069,16 @@
         <v>31</v>
       </c>
       <c r="B57" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
       </c>
       <c r="D57" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E57" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2086,16 +2086,16 @@
         <v>31</v>
       </c>
       <c r="B58" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C58" t="s">
         <v>6</v>
       </c>
       <c r="D58" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2103,16 +2103,16 @@
         <v>31</v>
       </c>
       <c r="B59" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C59" t="s">
         <v>6</v>
       </c>
       <c r="D59" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2120,16 +2120,16 @@
         <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C60" t="s">
         <v>6</v>
       </c>
       <c r="D60" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E60" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2137,16 +2137,16 @@
         <v>31</v>
       </c>
       <c r="B61" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C61" t="s">
         <v>6</v>
       </c>
       <c r="D61" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2154,16 +2154,16 @@
         <v>31</v>
       </c>
       <c r="B62" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D62" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E62" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2171,16 +2171,16 @@
         <v>31</v>
       </c>
       <c r="B63" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C63" t="s">
         <v>6</v>
       </c>
       <c r="D63" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E63" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2222,13 +2222,13 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
+        <v>167</v>
+      </c>
+      <c r="C66" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" t="s">
         <v>168</v>
-      </c>
-      <c r="C66" t="s">
-        <v>6</v>
-      </c>
-      <c r="D66" t="s">
-        <v>169</v>
       </c>
       <c r="E66" t="s">
         <v>15</v>
@@ -2236,16 +2236,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>162</v>
+      </c>
+      <c r="B67" t="s">
         <v>163</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" t="s">
         <v>164</v>
-      </c>
-      <c r="C67" t="s">
-        <v>6</v>
-      </c>
-      <c r="D67" t="s">
-        <v>165</v>
       </c>
       <c r="E67" t="s">
         <v>15</v>
@@ -2253,16 +2253,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>60</v>
+      </c>
+      <c r="B68" t="s">
         <v>61</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>62</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>63</v>
-      </c>
-      <c r="D68" t="s">
-        <v>64</v>
       </c>
       <c r="E68" t="s">
         <v>15</v>
@@ -2270,16 +2270,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>206</v>
+      </c>
+      <c r="B69" t="s">
+        <v>207</v>
+      </c>
+      <c r="C69" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" t="s">
         <v>208</v>
-      </c>
-      <c r="B69" t="s">
-        <v>209</v>
-      </c>
-      <c r="C69" t="s">
-        <v>6</v>
-      </c>
-      <c r="D69" t="s">
-        <v>210</v>
       </c>
       <c r="E69" t="s">
         <v>15</v>
@@ -2287,16 +2287,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>136</v>
+      </c>
+      <c r="B70" t="s">
         <v>137</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" t="s">
         <v>138</v>
-      </c>
-      <c r="C70" t="s">
-        <v>6</v>
-      </c>
-      <c r="D70" t="s">
-        <v>139</v>
       </c>
       <c r="E70" t="s">
         <v>15</v>
@@ -2304,16 +2304,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B71" t="s">
+        <v>139</v>
+      </c>
+      <c r="C71" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" t="s">
         <v>140</v>
-      </c>
-      <c r="C71" t="s">
-        <v>6</v>
-      </c>
-      <c r="D71" t="s">
-        <v>141</v>
       </c>
       <c r="E71" t="s">
         <v>15</v>
@@ -2321,16 +2321,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>98</v>
+      </c>
+      <c r="B72" t="s">
         <v>99</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" t="s">
         <v>100</v>
-      </c>
-      <c r="C72" t="s">
-        <v>6</v>
-      </c>
-      <c r="D72" t="s">
-        <v>101</v>
       </c>
       <c r="E72" t="s">
         <v>15</v>
@@ -2338,16 +2338,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>147</v>
+      </c>
+      <c r="B73" t="s">
         <v>148</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
+        <v>68</v>
+      </c>
+      <c r="D73" t="s">
         <v>149</v>
-      </c>
-      <c r="C73" t="s">
-        <v>69</v>
-      </c>
-      <c r="D73" t="s">
-        <v>150</v>
       </c>
       <c r="E73" t="s">
         <v>15</v>
@@ -2375,13 +2375,13 @@
         <v>10</v>
       </c>
       <c r="B75" t="s">
+        <v>101</v>
+      </c>
+      <c r="C75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" t="s">
         <v>102</v>
-      </c>
-      <c r="C75" t="s">
-        <v>6</v>
-      </c>
-      <c r="D75" t="s">
-        <v>103</v>
       </c>
       <c r="E75" t="s">
         <v>15</v>
@@ -2392,13 +2392,13 @@
         <v>10</v>
       </c>
       <c r="B76" t="s">
+        <v>175</v>
+      </c>
+      <c r="C76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" t="s">
         <v>176</v>
-      </c>
-      <c r="C76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76" t="s">
-        <v>177</v>
       </c>
       <c r="E76" t="s">
         <v>15</v>
@@ -2409,13 +2409,13 @@
         <v>10</v>
       </c>
       <c r="B77" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
       </c>
       <c r="D77" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E77" t="s">
         <v>15</v>
@@ -2460,13 +2460,13 @@
         <v>22</v>
       </c>
       <c r="B80" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
       </c>
       <c r="D80" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E80" t="s">
         <v>15</v>
@@ -2477,13 +2477,13 @@
         <v>22</v>
       </c>
       <c r="B81" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C81" t="s">
         <v>6</v>
       </c>
       <c r="D81" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E81" t="s">
         <v>15</v>
@@ -2491,16 +2491,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82" t="s">
         <v>88</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82" t="s">
         <v>89</v>
-      </c>
-      <c r="C82" t="s">
-        <v>6</v>
-      </c>
-      <c r="D82" t="s">
-        <v>90</v>
       </c>
       <c r="E82" t="s">
         <v>15</v>
@@ -2508,16 +2508,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B83" t="s">
+        <v>165</v>
+      </c>
+      <c r="C83" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" t="s">
         <v>166</v>
-      </c>
-      <c r="C83" t="s">
-        <v>6</v>
-      </c>
-      <c r="D83" t="s">
-        <v>167</v>
       </c>
       <c r="E83" t="s">
         <v>15</v>
@@ -2525,16 +2525,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B84" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C84" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D84" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E84" t="s">
         <v>15</v>
@@ -2542,16 +2542,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>141</v>
+      </c>
+      <c r="B85" t="s">
         <v>142</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" t="s">
         <v>143</v>
-      </c>
-      <c r="C85" t="s">
-        <v>6</v>
-      </c>
-      <c r="D85" t="s">
-        <v>144</v>
       </c>
       <c r="E85" t="s">
         <v>15</v>
@@ -2559,16 +2559,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>144</v>
+      </c>
+      <c r="B86" t="s">
         <v>145</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
+        <v>68</v>
+      </c>
+      <c r="D86" t="s">
         <v>146</v>
-      </c>
-      <c r="C86" t="s">
-        <v>69</v>
-      </c>
-      <c r="D86" t="s">
-        <v>147</v>
       </c>
       <c r="E86" t="s">
         <v>15</v>
@@ -2596,13 +2596,13 @@
         <v>28</v>
       </c>
       <c r="B88" t="s">
+        <v>78</v>
+      </c>
+      <c r="C88" t="s">
+        <v>6</v>
+      </c>
+      <c r="D88" t="s">
         <v>79</v>
-      </c>
-      <c r="C88" t="s">
-        <v>6</v>
-      </c>
-      <c r="D88" t="s">
-        <v>80</v>
       </c>
       <c r="E88" t="s">
         <v>15</v>
@@ -2613,13 +2613,13 @@
         <v>28</v>
       </c>
       <c r="B89" t="s">
+        <v>85</v>
+      </c>
+      <c r="C89" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" t="s">
         <v>86</v>
-      </c>
-      <c r="C89" t="s">
-        <v>6</v>
-      </c>
-      <c r="D89" t="s">
-        <v>87</v>
       </c>
       <c r="E89" t="s">
         <v>15</v>
@@ -2630,13 +2630,13 @@
         <v>28</v>
       </c>
       <c r="B90" t="s">
+        <v>169</v>
+      </c>
+      <c r="C90" t="s">
+        <v>6</v>
+      </c>
+      <c r="D90" t="s">
         <v>170</v>
-      </c>
-      <c r="C90" t="s">
-        <v>6</v>
-      </c>
-      <c r="D90" t="s">
-        <v>171</v>
       </c>
       <c r="E90" t="s">
         <v>15</v>
@@ -2647,13 +2647,13 @@
         <v>28</v>
       </c>
       <c r="B91" t="s">
+        <v>171</v>
+      </c>
+      <c r="C91" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" t="s">
         <v>172</v>
-      </c>
-      <c r="C91" t="s">
-        <v>6</v>
-      </c>
-      <c r="D91" t="s">
-        <v>173</v>
       </c>
       <c r="E91" t="s">
         <v>15</v>
@@ -2661,16 +2661,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>57</v>
+      </c>
+      <c r="B92" t="s">
         <v>58</v>
-      </c>
-      <c r="B92" t="s">
-        <v>59</v>
       </c>
       <c r="C92" t="s">
         <v>27</v>
       </c>
       <c r="D92" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E92" t="s">
         <v>15</v>
@@ -2678,16 +2678,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B93" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C93" t="s">
         <v>27</v>
       </c>
       <c r="D93" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E93" t="s">
         <v>15</v>
@@ -2695,16 +2695,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B94" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C94" t="s">
         <v>27</v>
       </c>
       <c r="D94" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E94" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Add Italia & India into website
</commit_message>
<xml_diff>
--- a/httpget/List File.xlsx
+++ b/httpget/List File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\script-nsg\httpget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7AEE07-08DB-4D6C-9820-998452E4F4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFDB17C-5F90-459B-9FB6-F8E1CB903E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{DC6502BA-425D-411E-B718-7BD70301C676}"/>
   </bookViews>
@@ -1002,10 +1002,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.72043010752688175</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.27956989247311825</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2133,7 +2133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C18607A-68F6-4C8B-BF40-82CCB3747CF3}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
       <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
@@ -2164,7 +2164,7 @@
       </c>
       <c r="H1" s="1">
         <f>COUNTIF(E:E,"Yes")/SUM(COUNTIF(E:E,"Yes"),COUNTIF(E:E,"No"))</f>
-        <v>0.66666666666666663</v>
+        <v>0.72043010752688175</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="H2" s="1">
         <f>COUNTIF(E:E,"No")/SUM(COUNTIF(E:E,"Yes"),COUNTIF(E:E,"No"))</f>
-        <v>0.33333333333333331</v>
+        <v>0.27956989247311825</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3242,7 +3242,7 @@
         <v>19</v>
       </c>
       <c r="E64" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3259,7 +3259,7 @@
         <v>224</v>
       </c>
       <c r="E65" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3276,7 +3276,7 @@
         <v>168</v>
       </c>
       <c r="E66" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3293,7 +3293,7 @@
         <v>164</v>
       </c>
       <c r="E67" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3310,7 +3310,7 @@
         <v>63</v>
       </c>
       <c r="E68" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add Latvia and Morocco to Website
</commit_message>
<xml_diff>
--- a/httpget/List File.xlsx
+++ b/httpget/List File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\script-nsg\httpget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFDB17C-5F90-459B-9FB6-F8E1CB903E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BB102A-6631-48E6-9CC0-30CD21D94EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{DC6502BA-425D-411E-B718-7BD70301C676}"/>
   </bookViews>
@@ -1002,10 +1002,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.72043010752688175</c:v>
+                  <c:v>0.75268817204301075</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.27956989247311825</c:v>
+                  <c:v>0.24731182795698925</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2134,7 +2134,7 @@
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+      <selection activeCell="E69" sqref="E69:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2164,7 +2164,7 @@
       </c>
       <c r="H1" s="1">
         <f>COUNTIF(E:E,"Yes")/SUM(COUNTIF(E:E,"Yes"),COUNTIF(E:E,"No"))</f>
-        <v>0.72043010752688175</v>
+        <v>0.75268817204301075</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="H2" s="1">
         <f>COUNTIF(E:E,"No")/SUM(COUNTIF(E:E,"Yes"),COUNTIF(E:E,"No"))</f>
-        <v>0.27956989247311825</v>
+        <v>0.24731182795698925</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3327,7 +3327,7 @@
         <v>208</v>
       </c>
       <c r="E69" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3344,7 +3344,7 @@
         <v>138</v>
       </c>
       <c r="E70" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3361,7 +3361,7 @@
         <v>140</v>
       </c>
       <c r="E71" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update 1 filename + xlsx + creation PDF
</commit_message>
<xml_diff>
--- a/httpget/List File.xlsx
+++ b/httpget/List File.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\script-nsg\httpget\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\git\script-nsg\httpget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BB102A-6631-48E6-9CC0-30CD21D94EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB61ADF-45B6-444F-96A5-DA3F1591CE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{DC6502BA-425D-411E-B718-7BD70301C676}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="251">
   <si>
     <t>Country</t>
   </si>
@@ -711,13 +711,91 @@
   </si>
   <si>
     <t>AmazonS3_eu-west-2_GB.xml</t>
+  </si>
+  <si>
+    <t>Bunny CDN</t>
+  </si>
+  <si>
+    <t>Bunny_CDN.xml</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>ICSCoE</t>
+  </si>
+  <si>
+    <t>ICSCoE_100Gbps_JP.xml</t>
+  </si>
+  <si>
+    <t>Iomart Leicester</t>
+  </si>
+  <si>
+    <t>Iomart Maidenhead</t>
+  </si>
+  <si>
+    <t>Iomart Nottingham</t>
+  </si>
+  <si>
+    <t>Iomart_10Gbps_Leicester_GB.xml</t>
+  </si>
+  <si>
+    <t>Iomart_10Gbps_Maidenhead_GB.xml</t>
+  </si>
+  <si>
+    <t>Iomart_10Gbps_Nottingham_GB.xml</t>
+  </si>
+  <si>
+    <t>Multacom LA</t>
+  </si>
+  <si>
+    <t>100Mbps</t>
+  </si>
+  <si>
+    <t>Multacom_100Mbps_LA_US.xml</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>RackRay</t>
+  </si>
+  <si>
+    <t>RackRay_1Gbps_Vilnius_LT.xml</t>
+  </si>
+  <si>
+    <t>Syntis SARL</t>
+  </si>
+  <si>
+    <t>Syntis SARL_10Gbps_Bordeaux_FR.xml</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>TOP 37</t>
+  </si>
+  <si>
+    <t>TOP 37_20Gbps_BR.xml</t>
+  </si>
+  <si>
+    <t>Velia</t>
+  </si>
+  <si>
+    <t>Velia_10Gbps_Strasbourg_FR.xml</t>
+  </si>
+  <si>
+    <t>Yamagata University</t>
+  </si>
+  <si>
+    <t>Yamagata University_10Gbps_Yamagata_JP.xml</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -728,6 +806,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -754,9 +838,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -891,6 +976,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-77B9-4044-A506-DDF7EB96B894}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -910,6 +1000,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-77B9-4044-A506-DDF7EB96B894}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1002,10 +1097,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.75268817204301075</c:v>
+                  <c:v>0.68269230769230771</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24731182795698925</c:v>
+                  <c:v>0.31730769230769229</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1785,7 +1880,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2131,10 +2226,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C18607A-68F6-4C8B-BF40-82CCB3747CF3}">
-  <dimension ref="A1:H94"/>
+  <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69:E71"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2164,7 +2259,7 @@
       </c>
       <c r="H1" s="1">
         <f>COUNTIF(E:E,"Yes")/SUM(COUNTIF(E:E,"Yes"),COUNTIF(E:E,"No"))</f>
-        <v>0.75268817204301075</v>
+        <v>0.68269230769230771</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2188,7 +2283,7 @@
       </c>
       <c r="H2" s="1">
         <f>COUNTIF(E:E,"No")/SUM(COUNTIF(E:E,"Yes"),COUNTIF(E:E,"No"))</f>
-        <v>0.24731182795698925</v>
+        <v>0.31730769230769229</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2261,33 +2356,33 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>244</v>
       </c>
       <c r="B7" t="s">
-        <v>155</v>
+        <v>245</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>154</v>
+        <v>246</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>153</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>155</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>218</v>
+        <v>154</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -2298,13 +2393,13 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>173</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>174</v>
+        <v>218</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -2312,16 +2407,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>104</v>
+        <v>173</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
-        <v>105</v>
+        <v>174</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -2329,16 +2424,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>105</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
@@ -2349,13 +2444,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
@@ -2366,13 +2461,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -2380,16 +2475,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="E14" t="s">
         <v>14</v>
@@ -2400,13 +2495,13 @@
         <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
         <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
         <v>14</v>
@@ -2414,16 +2509,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>221</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
         <v>14</v>
@@ -2434,13 +2529,13 @@
         <v>106</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>109</v>
+        <v>221</v>
       </c>
       <c r="E17" t="s">
         <v>14</v>
@@ -2451,13 +2546,13 @@
         <v>106</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E18" t="s">
         <v>14</v>
@@ -2468,13 +2563,13 @@
         <v>106</v>
       </c>
       <c r="B19" t="s">
-        <v>219</v>
+        <v>110</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E19" t="s">
         <v>14</v>
@@ -2485,13 +2580,13 @@
         <v>106</v>
       </c>
       <c r="B20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C20" t="s">
         <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E20" t="s">
         <v>14</v>
@@ -2499,16 +2594,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>220</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="E21" t="s">
         <v>14</v>
@@ -2516,16 +2611,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="E22" t="s">
         <v>14</v>
@@ -2536,13 +2631,13 @@
         <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E23" t="s">
         <v>14</v>
@@ -2553,13 +2648,13 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E24" t="s">
         <v>14</v>
@@ -2570,13 +2665,13 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E25" t="s">
         <v>14</v>
@@ -2587,13 +2682,13 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E26" t="s">
         <v>14</v>
@@ -2604,13 +2699,13 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E27" t="s">
         <v>14</v>
@@ -2621,13 +2716,13 @@
         <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E28" t="s">
         <v>14</v>
@@ -2638,13 +2733,13 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E29" t="s">
         <v>14</v>
@@ -2655,13 +2750,13 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E30" t="s">
         <v>14</v>
@@ -2672,13 +2767,13 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>222</v>
+        <v>49</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E31" t="s">
         <v>14</v>
@@ -2689,13 +2784,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>74</v>
+        <v>222</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="E32" t="s">
         <v>14</v>
@@ -2706,13 +2801,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E33" t="s">
         <v>14</v>
@@ -2723,13 +2818,13 @@
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="E34" t="s">
         <v>14</v>
@@ -2740,13 +2835,13 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E35" t="s">
         <v>14</v>
@@ -2757,13 +2852,13 @@
         <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E36" t="s">
         <v>14</v>
@@ -2774,13 +2869,13 @@
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D37" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="E37" t="s">
         <v>14</v>
@@ -2791,13 +2886,13 @@
         <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E38" t="s">
         <v>14</v>
@@ -2808,13 +2903,13 @@
         <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E39" t="s">
         <v>14</v>
@@ -2825,13 +2920,13 @@
         <v>31</v>
       </c>
       <c r="B40" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E40" t="s">
         <v>14</v>
@@ -2842,13 +2937,13 @@
         <v>31</v>
       </c>
       <c r="B41" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E41" t="s">
         <v>14</v>
@@ -2859,13 +2954,13 @@
         <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E42" t="s">
         <v>14</v>
@@ -2876,13 +2971,13 @@
         <v>31</v>
       </c>
       <c r="B43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E43" t="s">
         <v>14</v>
@@ -2893,13 +2988,13 @@
         <v>31</v>
       </c>
       <c r="B44" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
       </c>
       <c r="D44" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E44" t="s">
         <v>14</v>
@@ -2910,13 +3005,13 @@
         <v>31</v>
       </c>
       <c r="B45" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E45" t="s">
         <v>14</v>
@@ -2927,13 +3022,13 @@
         <v>31</v>
       </c>
       <c r="B46" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
       </c>
       <c r="D46" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E46" t="s">
         <v>14</v>
@@ -2944,13 +3039,13 @@
         <v>31</v>
       </c>
       <c r="B47" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
       </c>
       <c r="D47" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E47" t="s">
         <v>14</v>
@@ -2961,13 +3056,13 @@
         <v>31</v>
       </c>
       <c r="B48" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="E48" t="s">
         <v>14</v>
@@ -2978,13 +3073,13 @@
         <v>31</v>
       </c>
       <c r="B49" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C49" t="s">
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E49" t="s">
         <v>14</v>
@@ -2995,13 +3090,13 @@
         <v>31</v>
       </c>
       <c r="B50" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C50" t="s">
         <v>6</v>
       </c>
       <c r="D50" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E50" t="s">
         <v>14</v>
@@ -3012,13 +3107,13 @@
         <v>31</v>
       </c>
       <c r="B51" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="C51" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D51" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="E51" t="s">
         <v>14</v>
@@ -3029,13 +3124,13 @@
         <v>31</v>
       </c>
       <c r="B52" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C52" t="s">
         <v>62</v>
       </c>
       <c r="D52" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E52" t="s">
         <v>14</v>
@@ -3046,13 +3141,13 @@
         <v>31</v>
       </c>
       <c r="B53" t="s">
-        <v>223</v>
+        <v>179</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D53" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E53" t="s">
         <v>14</v>
@@ -3063,13 +3158,13 @@
         <v>31</v>
       </c>
       <c r="B54" t="s">
-        <v>184</v>
+        <v>223</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
       </c>
       <c r="D54" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E54" t="s">
         <v>14</v>
@@ -3080,13 +3175,13 @@
         <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E55" t="s">
         <v>14</v>
@@ -3097,13 +3192,13 @@
         <v>31</v>
       </c>
       <c r="B56" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
       </c>
       <c r="D56" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E56" t="s">
         <v>14</v>
@@ -3114,13 +3209,13 @@
         <v>31</v>
       </c>
       <c r="B57" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
       </c>
       <c r="D57" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E57" t="s">
         <v>14</v>
@@ -3131,13 +3226,13 @@
         <v>31</v>
       </c>
       <c r="B58" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C58" t="s">
         <v>6</v>
       </c>
       <c r="D58" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E58" t="s">
         <v>14</v>
@@ -3148,13 +3243,13 @@
         <v>31</v>
       </c>
       <c r="B59" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C59" t="s">
         <v>6</v>
       </c>
       <c r="D59" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E59" t="s">
         <v>14</v>
@@ -3165,13 +3260,13 @@
         <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C60" t="s">
         <v>6</v>
       </c>
       <c r="D60" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E60" t="s">
         <v>14</v>
@@ -3182,13 +3277,13 @@
         <v>31</v>
       </c>
       <c r="B61" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C61" t="s">
         <v>6</v>
       </c>
       <c r="D61" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E61" t="s">
         <v>14</v>
@@ -3199,13 +3294,13 @@
         <v>31</v>
       </c>
       <c r="B62" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C62" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D62" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E62" t="s">
         <v>14</v>
@@ -3216,13 +3311,13 @@
         <v>31</v>
       </c>
       <c r="B63" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D63" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E63" t="s">
         <v>14</v>
@@ -3230,16 +3325,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B64" t="s">
-        <v>18</v>
+        <v>202</v>
       </c>
       <c r="C64" t="s">
         <v>6</v>
       </c>
       <c r="D64" t="s">
-        <v>19</v>
+        <v>203</v>
       </c>
       <c r="E64" t="s">
         <v>14</v>
@@ -3247,16 +3342,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B65" t="s">
-        <v>26</v>
+        <v>242</v>
       </c>
       <c r="C65" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D65" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="E65" t="s">
         <v>14</v>
@@ -3264,33 +3359,33 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B66" t="s">
-        <v>167</v>
+        <v>247</v>
       </c>
       <c r="C66" t="s">
         <v>6</v>
       </c>
       <c r="D66" t="s">
-        <v>168</v>
+        <v>248</v>
       </c>
       <c r="E66" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>162</v>
+        <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>163</v>
+        <v>18</v>
       </c>
       <c r="C67" t="s">
         <v>6</v>
       </c>
       <c r="D67" t="s">
-        <v>164</v>
+        <v>19</v>
       </c>
       <c r="E67" t="s">
         <v>14</v>
@@ -3298,16 +3393,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="B68" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="C68" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="D68" t="s">
-        <v>63</v>
+        <v>224</v>
       </c>
       <c r="E68" t="s">
         <v>14</v>
@@ -3315,118 +3410,118 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>206</v>
+        <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>207</v>
+        <v>230</v>
       </c>
       <c r="C69" t="s">
         <v>6</v>
       </c>
       <c r="D69" t="s">
-        <v>208</v>
+        <v>233</v>
       </c>
       <c r="E69" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>136</v>
+        <v>17</v>
       </c>
       <c r="B70" t="s">
-        <v>137</v>
+        <v>231</v>
       </c>
       <c r="C70" t="s">
         <v>6</v>
       </c>
       <c r="D70" t="s">
-        <v>138</v>
+        <v>234</v>
       </c>
       <c r="E70" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>136</v>
+        <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>139</v>
+        <v>232</v>
       </c>
       <c r="C71" t="s">
         <v>6</v>
       </c>
       <c r="D71" t="s">
-        <v>140</v>
+        <v>235</v>
       </c>
       <c r="E71" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="B72" t="s">
-        <v>99</v>
+        <v>167</v>
       </c>
       <c r="C72" t="s">
         <v>6</v>
       </c>
       <c r="D72" t="s">
-        <v>100</v>
+        <v>168</v>
       </c>
       <c r="E72" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="B73" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="C73" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="D73" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="E73" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="B74" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="C74" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D74" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="E74" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>10</v>
+        <v>227</v>
       </c>
       <c r="B75" t="s">
-        <v>101</v>
+        <v>228</v>
       </c>
       <c r="C75" t="s">
-        <v>6</v>
-      </c>
-      <c r="D75" t="s">
-        <v>102</v>
+        <v>62</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>229</v>
       </c>
       <c r="E75" t="s">
         <v>15</v>
@@ -3434,16 +3529,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>10</v>
+        <v>227</v>
       </c>
       <c r="B76" t="s">
-        <v>175</v>
+        <v>249</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
       </c>
-      <c r="D76" t="s">
-        <v>176</v>
+      <c r="D76" s="2" t="s">
+        <v>250</v>
       </c>
       <c r="E76" t="s">
         <v>15</v>
@@ -3451,16 +3546,16 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>10</v>
+        <v>239</v>
       </c>
       <c r="B77" t="s">
-        <v>182</v>
+        <v>240</v>
       </c>
       <c r="C77" t="s">
-        <v>6</v>
-      </c>
-      <c r="D77" t="s">
-        <v>183</v>
+        <v>68</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>241</v>
       </c>
       <c r="E77" t="s">
         <v>15</v>
@@ -3468,67 +3563,67 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>22</v>
+        <v>206</v>
       </c>
       <c r="B78" t="s">
-        <v>35</v>
+        <v>207</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
       </c>
       <c r="D78" t="s">
-        <v>36</v>
+        <v>208</v>
       </c>
       <c r="E78" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>22</v>
+        <v>136</v>
       </c>
       <c r="B79" t="s">
-        <v>23</v>
+        <v>137</v>
       </c>
       <c r="C79" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D79" t="s">
-        <v>25</v>
+        <v>138</v>
       </c>
       <c r="E79" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>22</v>
+        <v>136</v>
       </c>
       <c r="B80" t="s">
-        <v>210</v>
+        <v>139</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
       </c>
       <c r="D80" t="s">
-        <v>209</v>
+        <v>140</v>
       </c>
       <c r="E80" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="B81" t="s">
-        <v>211</v>
+        <v>99</v>
       </c>
       <c r="C81" t="s">
         <v>6</v>
       </c>
       <c r="D81" t="s">
-        <v>212</v>
+        <v>100</v>
       </c>
       <c r="E81" t="s">
         <v>15</v>
@@ -3536,16 +3631,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>87</v>
+        <v>147</v>
       </c>
       <c r="B82" t="s">
-        <v>88</v>
+        <v>148</v>
       </c>
       <c r="C82" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="D82" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="E82" t="s">
         <v>15</v>
@@ -3553,16 +3648,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>87</v>
+        <v>10</v>
       </c>
       <c r="B83" t="s">
-        <v>165</v>
+        <v>9</v>
       </c>
       <c r="C83" t="s">
         <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>166</v>
+        <v>8</v>
       </c>
       <c r="E83" t="s">
         <v>15</v>
@@ -3570,16 +3665,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>87</v>
+        <v>10</v>
       </c>
       <c r="B84" t="s">
-        <v>213</v>
+        <v>101</v>
       </c>
       <c r="C84" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="D84" t="s">
-        <v>214</v>
+        <v>102</v>
       </c>
       <c r="E84" t="s">
         <v>15</v>
@@ -3587,16 +3682,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>141</v>
+        <v>10</v>
       </c>
       <c r="B85" t="s">
-        <v>142</v>
+        <v>175</v>
       </c>
       <c r="C85" t="s">
         <v>6</v>
       </c>
       <c r="D85" t="s">
-        <v>143</v>
+        <v>176</v>
       </c>
       <c r="E85" t="s">
         <v>15</v>
@@ -3604,16 +3699,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>144</v>
+        <v>10</v>
       </c>
       <c r="B86" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="C86" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="D86" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
       <c r="E86" t="s">
         <v>15</v>
@@ -3621,16 +3716,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B87" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C87" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D87" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E87" t="s">
         <v>15</v>
@@ -3638,16 +3733,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B88" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="C88" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D88" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="E88" t="s">
         <v>15</v>
@@ -3655,16 +3750,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B89" t="s">
-        <v>85</v>
+        <v>210</v>
       </c>
       <c r="C89" t="s">
         <v>6</v>
       </c>
       <c r="D89" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
       <c r="E89" t="s">
         <v>15</v>
@@ -3672,16 +3767,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B90" t="s">
-        <v>169</v>
+        <v>211</v>
       </c>
       <c r="C90" t="s">
         <v>6</v>
       </c>
       <c r="D90" t="s">
-        <v>170</v>
+        <v>212</v>
       </c>
       <c r="E90" t="s">
         <v>15</v>
@@ -3689,16 +3784,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="B91" t="s">
-        <v>171</v>
+        <v>88</v>
       </c>
       <c r="C91" t="s">
         <v>6</v>
       </c>
       <c r="D91" t="s">
-        <v>172</v>
+        <v>89</v>
       </c>
       <c r="E91" t="s">
         <v>15</v>
@@ -3706,16 +3801,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="B92" t="s">
-        <v>58</v>
+        <v>165</v>
       </c>
       <c r="C92" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D92" t="s">
-        <v>59</v>
+        <v>166</v>
       </c>
       <c r="E92" t="s">
         <v>15</v>
@@ -3723,16 +3818,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="B93" t="s">
-        <v>72</v>
+        <v>213</v>
       </c>
       <c r="C93" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="D93" t="s">
-        <v>73</v>
+        <v>214</v>
       </c>
       <c r="E93" t="s">
         <v>15</v>
@@ -3740,18 +3835,205 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>141</v>
+      </c>
+      <c r="B94" t="s">
+        <v>142</v>
+      </c>
+      <c r="C94" t="s">
+        <v>6</v>
+      </c>
+      <c r="D94" t="s">
+        <v>143</v>
+      </c>
+      <c r="E94" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>144</v>
+      </c>
+      <c r="B95" t="s">
+        <v>145</v>
+      </c>
+      <c r="C95" t="s">
+        <v>68</v>
+      </c>
+      <c r="D95" t="s">
+        <v>146</v>
+      </c>
+      <c r="E95" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>28</v>
+      </c>
+      <c r="B96" t="s">
+        <v>29</v>
+      </c>
+      <c r="C96" t="s">
+        <v>27</v>
+      </c>
+      <c r="D96" t="s">
+        <v>30</v>
+      </c>
+      <c r="E96" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>28</v>
+      </c>
+      <c r="B97" t="s">
+        <v>78</v>
+      </c>
+      <c r="C97" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" t="s">
+        <v>79</v>
+      </c>
+      <c r="E97" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>28</v>
+      </c>
+      <c r="B98" t="s">
+        <v>85</v>
+      </c>
+      <c r="C98" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" t="s">
+        <v>86</v>
+      </c>
+      <c r="E98" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>28</v>
+      </c>
+      <c r="B99" t="s">
+        <v>236</v>
+      </c>
+      <c r="C99" t="s">
+        <v>237</v>
+      </c>
+      <c r="D99" t="s">
+        <v>238</v>
+      </c>
+      <c r="E99" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>28</v>
+      </c>
+      <c r="B100" t="s">
+        <v>169</v>
+      </c>
+      <c r="C100" t="s">
+        <v>6</v>
+      </c>
+      <c r="D100" t="s">
+        <v>170</v>
+      </c>
+      <c r="E100" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>28</v>
+      </c>
+      <c r="B101" t="s">
+        <v>171</v>
+      </c>
+      <c r="C101" t="s">
+        <v>6</v>
+      </c>
+      <c r="D101" t="s">
+        <v>172</v>
+      </c>
+      <c r="E101" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>57</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B102" t="s">
+        <v>58</v>
+      </c>
+      <c r="C102" t="s">
+        <v>27</v>
+      </c>
+      <c r="D102" t="s">
+        <v>59</v>
+      </c>
+      <c r="E102" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>57</v>
+      </c>
+      <c r="B103" t="s">
+        <v>72</v>
+      </c>
+      <c r="C103" t="s">
+        <v>27</v>
+      </c>
+      <c r="D103" t="s">
+        <v>73</v>
+      </c>
+      <c r="E103" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>57</v>
+      </c>
+      <c r="B104" t="s">
         <v>94</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C104" t="s">
         <v>27</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D104" t="s">
         <v>95</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E104" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>57</v>
+      </c>
+      <c r="B105" t="s">
+        <v>225</v>
+      </c>
+      <c r="C105" t="s">
+        <v>27</v>
+      </c>
+      <c r="D105" t="s">
+        <v>226</v>
+      </c>
+      <c r="E105" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3765,6 +4047,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add new French server
</commit_message>
<xml_diff>
--- a/httpget/List File.xlsx
+++ b/httpget/List File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\git\script-nsg\httpget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EC5240-3AB8-4636-B4D5-9288258B177E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BE3E7F-6137-4EC7-9FC2-5A26CA49EAA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DC6502BA-425D-411E-B718-7BD70301C676}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{DC6502BA-425D-411E-B718-7BD70301C676}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1113,10 +1113,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.68269230769230771</c:v>
+                  <c:v>0.70192307692307687</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.31730769230769229</c:v>
+                  <c:v>0.29807692307692307</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2244,8 +2244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C18607A-68F6-4C8B-BF40-82CCB3747CF3}">
   <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2275,7 +2275,7 @@
       </c>
       <c r="H1" s="1">
         <f>COUNTIF(E:E,"Yes")/SUM(COUNTIF(E:E,"Yes"),COUNTIF(E:E,"No"))</f>
-        <v>0.68269230769230771</v>
+        <v>0.70192307692307687</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="H2" s="1">
         <f>COUNTIF(E:E,"No")/SUM(COUNTIF(E:E,"Yes"),COUNTIF(E:E,"No"))</f>
-        <v>0.31730769230769229</v>
+        <v>0.29807692307692307</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2384,7 +2384,7 @@
         <v>246</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3387,7 +3387,7 @@
         <v>248</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add LT & MC Server
</commit_message>
<xml_diff>
--- a/httpget/List File.xlsx
+++ b/httpget/List File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\git\script-nsg\httpget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FDDA70-C089-4F6E-A5CD-F82B8859EAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F4C839-7905-4A43-8BDA-C58DEF9A40EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{DC6502BA-425D-411E-B718-7BD70301C676}"/>
   </bookViews>
@@ -1113,10 +1113,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.75</c:v>
+                  <c:v>0.76923076923076927</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25</c:v>
+                  <c:v>0.23076923076923078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2244,8 +2244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C18607A-68F6-4C8B-BF40-82CCB3747CF3}">
   <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74:E76"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2275,7 +2275,7 @@
       </c>
       <c r="H1" s="1">
         <f>COUNTIF(E:E,"Yes")/SUM(COUNTIF(E:E,"Yes"),COUNTIF(E:E,"No"))</f>
-        <v>0.75</v>
+        <v>0.76923076923076927</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="H2" s="1">
         <f>COUNTIF(E:E,"No")/SUM(COUNTIF(E:E,"Yes"),COUNTIF(E:E,"No"))</f>
-        <v>0.25</v>
+        <v>0.23076923076923078</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3574,7 +3574,7 @@
         <v>241</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3642,7 +3642,7 @@
         <v>100</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Final Website (until new file)
</commit_message>
<xml_diff>
--- a/httpget/List File.xlsx
+++ b/httpget/List File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\git\script-nsg\httpget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDA5CF3-A500-400C-91EE-C44D64488C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7758F6F5-DFAA-4EA5-933F-9BE9394F0A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{DC6502BA-425D-411E-B718-7BD70301C676}"/>
   </bookViews>
@@ -1113,10 +1113,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.88461538461538458</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.11538461538461539</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2244,8 +2244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C18607A-68F6-4C8B-BF40-82CCB3747CF3}">
   <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90:E93"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101:E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2275,7 +2275,7 @@
       </c>
       <c r="H1" s="1">
         <f>COUNTIF(E:E,"Yes")/SUM(COUNTIF(E:E,"Yes"),COUNTIF(E:E,"No"))</f>
-        <v>0.88461538461538458</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="H2" s="1">
         <f>COUNTIF(E:E,"No")/SUM(COUNTIF(E:E,"Yes"),COUNTIF(E:E,"No"))</f>
-        <v>0.11538461538461539</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3863,7 +3863,7 @@
         <v>143</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3880,7 +3880,7 @@
         <v>146</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3897,7 +3897,7 @@
         <v>30</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3914,7 +3914,7 @@
         <v>79</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -3931,7 +3931,7 @@
         <v>86</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -3948,7 +3948,7 @@
         <v>238</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3965,7 +3965,7 @@
         <v>170</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3982,7 +3982,7 @@
         <v>172</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3990,16 +3990,16 @@
         <v>57</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>58</v>
+        <v>225</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>59</v>
+        <v>226</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -4007,16 +4007,16 @@
         <v>57</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -4024,16 +4024,16 @@
         <v>57</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -4041,16 +4041,16 @@
         <v>57</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>225</v>
+        <v>94</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>226</v>
+        <v>95</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more new server in file
</commit_message>
<xml_diff>
--- a/httpget/List File.xlsx
+++ b/httpget/List File.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\git\script-nsg\httpget\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://valentinslr-my.sharepoint.com/personal/hello_valentinslr_com/Documents/Documents/GitHub/script-nsg/httpget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D894E5D9-125F-427A-8D95-FE59EEB2AFA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{D894E5D9-125F-427A-8D95-FE59EEB2AFA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{551459F2-B13C-44F7-968F-BD4F9D857651}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{DC6502BA-425D-411E-B718-7BD70301C676}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="291">
   <si>
     <t>Country</t>
   </si>
@@ -822,6 +822,93 @@
   </si>
   <si>
     <t>Zero.com.ar_1Gbps_AR.xml</t>
+  </si>
+  <si>
+    <t>Orange MG</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>Orange B Evere</t>
+  </si>
+  <si>
+    <t>Orange B Evere_20Gbps_BE.xml</t>
+  </si>
+  <si>
+    <t>Orange B Hoboken</t>
+  </si>
+  <si>
+    <t>Orange B Hoboken_20Gbps_BE.xml</t>
+  </si>
+  <si>
+    <t>BF</t>
+  </si>
+  <si>
+    <t>Orange BF</t>
+  </si>
+  <si>
+    <t>Orange BF_10Gbps_BF.xml</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>Orange CI (Srv 1)</t>
+  </si>
+  <si>
+    <t>Orange CI (Srv 2)</t>
+  </si>
+  <si>
+    <t>Orange CI (Srv 1)_10Gbps_CI.xml</t>
+  </si>
+  <si>
+    <t>Orange CI (Srv 2)_10Gbps_CI.xml</t>
+  </si>
+  <si>
+    <t>Orange FR - Réunion</t>
+  </si>
+  <si>
+    <t>Orange F - Réunion_10Gbps_RE.xml</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>Orange MD</t>
+  </si>
+  <si>
+    <t>Orange MD_10Gbps_MD.xml</t>
+  </si>
+  <si>
+    <t>Orange MG_10Gbps_MG.xml</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>Orange RDC</t>
+  </si>
+  <si>
+    <t>Orange RDC_10Gbps_CD.xml</t>
+  </si>
+  <si>
+    <t>SFR GF Matoury</t>
+  </si>
+  <si>
+    <t>SFR GF Matoury_10Gbps_FR.xml</t>
+  </si>
+  <si>
+    <t>SFR MQ Le Lamentin</t>
+  </si>
+  <si>
+    <t>SFR MQ Le Lamentin_10Gbps_FR.xml</t>
+  </si>
+  <si>
+    <t>SRR (SFR Réunion)</t>
+  </si>
+  <si>
+    <t>SRR (SFR Réunion)_10Gbps_FR.xml</t>
   </si>
 </sst>
 </file>
@@ -1146,10 +1233,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.96296296296296291</c:v>
+                  <c:v>0.8666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.7037037037037035E-2</c:v>
+                  <c:v>0.13333333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1929,7 +2016,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2275,10 +2362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C18607A-68F6-4C8B-BF40-82CCB3747CF3}">
-  <dimension ref="A1:H109"/>
+  <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2308,7 +2395,7 @@
       </c>
       <c r="H1" s="1">
         <f>COUNTIF(E:E,"Yes")/SUM(COUNTIF(E:E,"Yes"),COUNTIF(E:E,"No"))</f>
-        <v>0.96296296296296291</v>
+        <v>0.8666666666666667</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2332,7 +2419,7 @@
       </c>
       <c r="H2" s="1">
         <f>COUNTIF(E:E,"No")/SUM(COUNTIF(E:E,"Yes"),COUNTIF(E:E,"No"))</f>
-        <v>3.7037037037037035E-2</v>
+        <v>0.13333333333333333</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2461,47 +2548,47 @@
         <v>215</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>216</v>
+        <v>264</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>217</v>
+        <v>265</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>245</v>
+        <v>266</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>246</v>
+        <v>267</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>153</v>
+        <v>215</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>155</v>
+        <v>216</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>154</v>
+        <v>217</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>14</v>
@@ -2509,33 +2596,33 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>268</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>21</v>
+        <v>269</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>218</v>
+        <v>270</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>244</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>173</v>
+        <v>245</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>174</v>
+        <v>246</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>14</v>
@@ -2543,16 +2630,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>103</v>
+        <v>153</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>104</v>
+        <v>155</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>105</v>
+        <v>154</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>14</v>
@@ -2560,33 +2647,33 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>11</v>
+        <v>282</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>12</v>
+        <v>283</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>16</v>
+        <v>284</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>65</v>
+        <v>218</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>14</v>
@@ -2594,16 +2681,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>80</v>
+        <v>173</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>81</v>
+        <v>174</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>14</v>
@@ -2611,50 +2698,50 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>66</v>
+        <v>271</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>67</v>
+        <v>272</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>69</v>
+        <v>274</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>66</v>
+        <v>271</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>70</v>
+        <v>273</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>71</v>
+        <v>275</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>221</v>
+        <v>105</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>14</v>
@@ -2662,16 +2749,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>109</v>
+        <v>16</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>14</v>
@@ -2679,16 +2766,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>110</v>
+        <v>64</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>111</v>
+        <v>65</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>14</v>
@@ -2696,16 +2783,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>219</v>
+        <v>80</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>14</v>
@@ -2713,16 +2800,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>220</v>
+        <v>67</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>14</v>
@@ -2730,16 +2817,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>14</v>
@@ -2747,16 +2834,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>34</v>
+        <v>221</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>14</v>
@@ -2764,16 +2851,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>37</v>
+        <v>108</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>38</v>
+        <v>109</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>14</v>
@@ -2781,16 +2868,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>14</v>
@@ -2798,16 +2885,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>41</v>
+        <v>219</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>14</v>
@@ -2815,16 +2902,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>52</v>
+        <v>220</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>53</v>
+        <v>113</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>14</v>
@@ -2832,16 +2919,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>14</v>
@@ -2852,13 +2939,13 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>14</v>
@@ -2869,13 +2956,13 @@
         <v>31</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>14</v>
@@ -2886,13 +2973,13 @@
         <v>31</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>14</v>
@@ -2903,13 +2990,13 @@
         <v>31</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>222</v>
+        <v>41</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>14</v>
@@ -2920,13 +3007,13 @@
         <v>31</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>14</v>
@@ -2937,13 +3024,13 @@
         <v>31</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>14</v>
@@ -2954,13 +3041,13 @@
         <v>31</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>14</v>
@@ -2971,13 +3058,13 @@
         <v>31</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>14</v>
@@ -2988,13 +3075,13 @@
         <v>31</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>14</v>
@@ -3005,13 +3092,13 @@
         <v>31</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>116</v>
+        <v>222</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>117</v>
+        <v>51</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>14</v>
@@ -3022,13 +3109,13 @@
         <v>31</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>119</v>
+        <v>75</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>14</v>
@@ -3039,13 +3126,13 @@
         <v>31</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>120</v>
+        <v>76</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>121</v>
+        <v>77</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>14</v>
@@ -3056,13 +3143,13 @@
         <v>31</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>14</v>
@@ -3073,13 +3160,13 @@
         <v>31</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>14</v>
@@ -3090,13 +3177,13 @@
         <v>31</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>14</v>
@@ -3107,13 +3194,13 @@
         <v>31</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>14</v>
@@ -3124,13 +3211,13 @@
         <v>31</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>14</v>
@@ -3141,13 +3228,13 @@
         <v>31</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>14</v>
@@ -3158,13 +3245,13 @@
         <v>31</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>14</v>
@@ -3175,13 +3262,13 @@
         <v>31</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>14</v>
@@ -3192,13 +3279,13 @@
         <v>31</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>157</v>
+        <v>125</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>14</v>
@@ -3209,13 +3296,13 @@
         <v>31</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>14</v>
@@ -3226,13 +3313,13 @@
         <v>31</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>14</v>
@@ -3243,13 +3330,13 @@
         <v>31</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>177</v>
+        <v>130</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>178</v>
+        <v>131</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>14</v>
@@ -3260,13 +3347,13 @@
         <v>31</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>179</v>
+        <v>132</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>180</v>
+        <v>133</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>14</v>
@@ -3277,16 +3364,16 @@
         <v>31</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>223</v>
+        <v>276</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>181</v>
+        <v>277</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -3294,13 +3381,13 @@
         <v>31</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>185</v>
+        <v>135</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>14</v>
@@ -3311,13 +3398,13 @@
         <v>31</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>14</v>
@@ -3328,13 +3415,13 @@
         <v>31</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>188</v>
+        <v>158</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>189</v>
+        <v>159</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>14</v>
@@ -3345,13 +3432,13 @@
         <v>31</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>191</v>
+        <v>161</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>14</v>
@@ -3362,13 +3449,13 @@
         <v>31</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>14</v>
@@ -3379,13 +3466,13 @@
         <v>31</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>14</v>
@@ -3396,13 +3483,13 @@
         <v>31</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>14</v>
@@ -3413,13 +3500,13 @@
         <v>31</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>14</v>
@@ -3430,13 +3517,13 @@
         <v>31</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>14</v>
@@ -3447,16 +3534,16 @@
         <v>31</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>202</v>
+        <v>285</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>203</v>
+        <v>286</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3464,13 +3551,13 @@
         <v>31</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>242</v>
+        <v>188</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>243</v>
+        <v>189</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>14</v>
@@ -3481,30 +3568,30 @@
         <v>31</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>247</v>
+        <v>287</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>248</v>
+        <v>288</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>18</v>
+        <v>190</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>19</v>
+        <v>191</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>14</v>
@@ -3512,16 +3599,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>26</v>
+        <v>192</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>224</v>
+        <v>193</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>14</v>
@@ -3529,16 +3616,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>230</v>
+        <v>194</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>233</v>
+        <v>195</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>14</v>
@@ -3546,16 +3633,16 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>231</v>
+        <v>196</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>234</v>
+        <v>197</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>14</v>
@@ -3563,16 +3650,16 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>232</v>
+        <v>198</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>235</v>
+        <v>199</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>14</v>
@@ -3580,16 +3667,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>168</v>
+        <v>201</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>14</v>
@@ -3597,16 +3684,16 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>162</v>
+        <v>31</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>163</v>
+        <v>202</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>164</v>
+        <v>203</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>14</v>
@@ -3614,33 +3701,33 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>61</v>
+        <v>289</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>63</v>
+        <v>290</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>227</v>
+        <v>31</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>229</v>
+        <v>6</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>14</v>
@@ -3648,16 +3735,16 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>227</v>
+        <v>31</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D80" s="3" t="s">
-        <v>250</v>
+      <c r="D80" s="2" t="s">
+        <v>248</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>14</v>
@@ -3665,16 +3752,16 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>239</v>
+        <v>17</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>240</v>
+        <v>18</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>241</v>
+        <v>6</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>14</v>
@@ -3682,16 +3769,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>206</v>
+        <v>17</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>207</v>
+        <v>26</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>14</v>
@@ -3699,16 +3786,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>136</v>
+        <v>17</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>138</v>
+        <v>233</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>14</v>
@@ -3716,16 +3803,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>136</v>
+        <v>17</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>139</v>
+        <v>231</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>140</v>
+        <v>234</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>14</v>
@@ -3733,16 +3820,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>99</v>
+        <v>232</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>100</v>
+        <v>235</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>14</v>
@@ -3750,16 +3837,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>147</v>
+        <v>17</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>14</v>
@@ -3767,16 +3854,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>10</v>
+        <v>162</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>8</v>
+        <v>164</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>14</v>
@@ -3784,16 +3871,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>14</v>
@@ -3801,16 +3888,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>10</v>
+        <v>227</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>175</v>
+        <v>228</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>176</v>
+        <v>62</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>229</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>14</v>
@@ -3818,16 +3905,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>10</v>
+        <v>227</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>182</v>
+        <v>249</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D90" s="2" t="s">
-        <v>183</v>
+      <c r="D90" s="3" t="s">
+        <v>250</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>14</v>
@@ -3835,16 +3922,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>22</v>
+        <v>239</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>35</v>
+        <v>240</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>36</v>
+        <v>68</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>241</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>14</v>
@@ -3852,16 +3939,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>22</v>
+        <v>206</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>23</v>
+        <v>207</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>25</v>
+        <v>208</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>14</v>
@@ -3869,16 +3956,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>22</v>
+        <v>136</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>210</v>
+        <v>137</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>209</v>
+        <v>138</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>14</v>
@@ -3886,16 +3973,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>22</v>
+        <v>136</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>211</v>
+        <v>139</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>212</v>
+        <v>140</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>14</v>
@@ -3903,16 +3990,16 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>14</v>
@@ -3920,50 +4007,50 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>87</v>
+        <v>278</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>165</v>
+        <v>279</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>166</v>
+        <v>280</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>87</v>
+        <v>263</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>213</v>
+        <v>262</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>214</v>
+        <v>281</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>14</v>
@@ -3971,16 +4058,16 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>144</v>
+        <v>10</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>145</v>
+        <v>9</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>146</v>
+        <v>8</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>14</v>
@@ -3988,16 +4075,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>14</v>
@@ -4005,16 +4092,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>78</v>
+        <v>175</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>14</v>
@@ -4022,16 +4109,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>85</v>
+        <v>182</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>86</v>
+        <v>183</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>14</v>
@@ -4039,16 +4126,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>236</v>
+        <v>35</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>237</v>
+        <v>6</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>238</v>
+        <v>36</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>14</v>
@@ -4056,16 +4143,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>169</v>
+        <v>23</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>170</v>
+        <v>25</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>14</v>
@@ -4073,16 +4160,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>171</v>
+        <v>210</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>172</v>
+        <v>209</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>14</v>
@@ -4090,16 +4177,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>14</v>
@@ -4107,16 +4194,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>14</v>
@@ -4124,16 +4211,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>72</v>
+        <v>165</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>73</v>
+        <v>166</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>14</v>
@@ -4141,18 +4228,222 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B118" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B121" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="C121" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D109" s="2" t="s">
+      <c r="D121" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E109" s="2" t="s">
+      <c r="E121" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>